<commit_message>
feat(BROWL): Base de dados
</commit_message>
<xml_diff>
--- a/docs/Estimativa de hrs.xlsx
+++ b/docs/Estimativa de hrs.xlsx
@@ -197,27 +197,27 @@
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,10 +513,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="1">
@@ -527,8 +527,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="9"/>
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="1">
@@ -536,8 +536,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="9"/>
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1">
@@ -548,197 +548,200 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>7</v>
+      <c r="A5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="C5" s="1">
         <v>2</v>
       </c>
-      <c r="D5" s="9" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
+      <c r="B8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2</v>
+      </c>
+      <c r="D10" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C11" s="1">
         <v>3</v>
       </c>
-      <c r="D6" s="9"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5" t="s">
+      <c r="D11" s="12"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C12" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="9"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5" t="s">
+      <c r="D12" s="12"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="C8" s="1">
-        <v>2</v>
-      </c>
-      <c r="D8" s="9"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="1">
-        <v>4</v>
-      </c>
-      <c r="D9" s="9"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="1">
-        <v>5</v>
-      </c>
-      <c r="D10" s="9"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="1">
-        <v>5</v>
-      </c>
-      <c r="D11" s="9"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>15</v>
       </c>
       <c r="C13" s="1">
         <v>2</v>
       </c>
+      <c r="D13" s="12"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7" t="s">
+      <c r="A14" s="10"/>
+      <c r="B14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="1">
+        <v>4</v>
+      </c>
+      <c r="D14" s="12"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="1">
+        <v>5</v>
+      </c>
+      <c r="D15" s="12"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="1">
+        <v>5</v>
+      </c>
+      <c r="D16" s="12"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+      <c r="B19" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C19" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="7" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="11"/>
+      <c r="B20" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C20" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
+      <c r="B21" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C21" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="7" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+      <c r="B22" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C22" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="7" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="11"/>
+      <c r="B23" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C23" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="8">
-        <f>SUM(C1:C23)</f>
+      <c r="C26" s="5">
+        <f>SUM(C1:C24)</f>
         <v>80</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D26" t="s">
         <v>28</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:A3"/>
-    <mergeCell ref="A5:A11"/>
-    <mergeCell ref="A13:A18"/>
-    <mergeCell ref="D5:D11"/>
-    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A10:A16"/>
+    <mergeCell ref="A18:A23"/>
+    <mergeCell ref="D10:D16"/>
+    <mergeCell ref="A5:A8"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>